<commit_message>
añadiendo el numero de corte al nombre del archivo
</commit_message>
<xml_diff>
--- a/coedicionesCOP.xlsx
+++ b/coedicionesCOP.xlsx
@@ -68,7 +68,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="[$$-240A]#,##0;[RED]\([$$-240A]#,##0\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -90,12 +90,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -217,7 +211,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -234,11 +228,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -354,9 +348,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1401840</xdr:colOff>
+      <xdr:colOff>1401480</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -370,7 +364,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="651240" y="533520"/>
-          <a:ext cx="750600" cy="746640"/>
+          <a:ext cx="750240" cy="746280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -392,12 +386,12 @@
   </sheetPr>
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="54" zoomScaleNormal="54" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
-      <selection pane="bottomRight" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>